<commit_message>
Adding some missing results
</commit_message>
<xml_diff>
--- a/data/2025-02-03/SCW Weekly Comp 2025-02-03 (Responses).xlsx
+++ b/data/2025-02-03/SCW Weekly Comp 2025-02-03 (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="234">
   <si>
     <t>Timestamp</t>
   </si>
@@ -704,6 +704,15 @@
   </si>
   <si>
     <t>3:09.79</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1662572041309805/permalink/1670925887141087/?app=fbl</t>
+  </si>
+  <si>
+    <t>27:17</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/595481126781396/permalink/605459715783537/?app=fbl</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1042,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:DF64" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:DF66" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="110">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -4215,44 +4224,114 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="17">
+      <c r="A64" s="12">
         <v>45705.138475590276</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C64" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D64" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E64" s="18" t="s">
+      <c r="E64" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F64" s="19" t="s">
+      <c r="F64" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="AC64" s="18" t="s">
+      <c r="AC64" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="AD64" s="18" t="s">
+      <c r="AD64" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="AE64" s="18" t="s">
+      <c r="AE64" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="AF64" s="18" t="s">
+      <c r="AF64" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="AG64" s="18" t="s">
+      <c r="AG64" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="AH64" s="18" t="s">
+      <c r="AH64" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="AI64" s="18" t="s">
+      <c r="AI64" s="13" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="9">
+        <v>45708.87036898149</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="DD65" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="DE65" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="DF65" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="17">
+        <v>45708.87219420139</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E66" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="O66" s="18">
+        <v>17.81</v>
+      </c>
+      <c r="P66" s="18">
+        <v>16.59</v>
+      </c>
+      <c r="Q66" s="18">
+        <v>18.51</v>
+      </c>
+      <c r="R66" s="18">
+        <v>19.04</v>
+      </c>
+      <c r="S66" s="18">
+        <v>20.04</v>
+      </c>
+      <c r="T66" s="18">
+        <v>16.59</v>
+      </c>
+      <c r="U66" s="18">
+        <v>18.45</v>
       </c>
     </row>
   </sheetData>
@@ -4320,10 +4399,12 @@
     <hyperlink r:id="rId61" ref="F62"/>
     <hyperlink r:id="rId62" ref="F63"/>
     <hyperlink r:id="rId63" ref="F64"/>
+    <hyperlink r:id="rId64" ref="F65"/>
+    <hyperlink r:id="rId65" ref="F66"/>
   </hyperlinks>
-  <drawing r:id="rId64"/>
+  <drawing r:id="rId66"/>
   <tableParts count="1">
-    <tablePart r:id="rId66"/>
+    <tablePart r:id="rId68"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>